<commit_message>
about page p'point slide
</commit_message>
<xml_diff>
--- a/Final report/Testing Spreadsheet v1.0 AboutPage.xlsx
+++ b/Final report/Testing Spreadsheet v1.0 AboutPage.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonnie\Documents\Software Development\CSC7056 Software Testing &amp; Verification\Group Project\Software-Testing-And-Verification\Final report\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <workbookProtection workbookPassword="A6C2" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="105" windowWidth="16560" windowHeight="6345" firstSheet="1" activeTab="2"/>
@@ -32,7 +27,7 @@
     <author>qubsys</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -70,7 +65,7 @@
     <author>qubsys</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -94,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -118,7 +113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -142,7 +137,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -166,7 +161,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1261,7 +1256,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1411,7 +1406,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1490,11 +1485,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1173210256"/>
-        <c:axId val="-1173212432"/>
+        <c:axId val="101920128"/>
+        <c:axId val="101926016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1173210256"/>
+        <c:axId val="101920128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1504,7 +1499,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1173212432"/>
+        <c:crossAx val="101926016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1512,7 +1507,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1173212432"/>
+        <c:axId val="101926016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1523,9 +1518,10 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1173210256"/>
+        <c:crossAx val="101920128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -1648,7 +1644,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1683,7 +1679,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1931,7 +1927,7 @@
   </sheetPr>
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -2252,8 +2248,8 @@
   </sheetPr>
   <dimension ref="A1:Z161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="AE27" sqref="AE27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5082,7 +5078,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView topLeftCell="A8" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5683,21 +5679,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0A86D0A1DF85A4CBF24319CD50F658E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18023c554c1e7c0fe5f8bda126dbbbe1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -5811,10 +5792,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
@@ -5829,16 +5832,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>